<commit_message>
Tidying up import function into TinyDB
</commit_message>
<xml_diff>
--- a/Beaconport Capture.xlsx
+++ b/Beaconport Capture.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://norfolksuffolkpolice-my.sharepoint.com/personal/patrick_thompson_norfolk_police_uk/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UserPC\Desktop\my_folder\Beaconport POC\beaconport_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{883918DD-E0D7-41D6-A1E4-67BDECAA8097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{955EC7C1-87CB-49C8-8D65-28AD6B6118C2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91C3BE2-7367-4424-BC9E-2E8C81871883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3BDA4877-5B23-49B1-ABB6-1AAF3516CA94}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{3BDA4877-5B23-49B1-ABB6-1AAF3516CA94}"/>
   </bookViews>
   <sheets>
     <sheet name="Beaconport Main" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <author>tc={311A7AA6-15CF-4FD5-9E87-9BAE24BC9A3F}</author>
   </authors>
   <commentList>
-    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{311A7AA6-15CF-4FD5-9E87-9BAE24BC9A3F}">
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{311A7AA6-15CF-4FD5-9E87-9BAE24BC9A3F}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="124">
   <si>
     <t>Offence Date</t>
   </si>
@@ -91,21 +91,12 @@
     <t>Force Code</t>
   </si>
   <si>
-    <t>CH1/001/2025</t>
-  </si>
-  <si>
     <t>Allocated To</t>
   </si>
   <si>
-    <t>Nominated Person</t>
-  </si>
-  <si>
     <t>36/12345/25</t>
   </si>
   <si>
-    <t>Narrative</t>
-  </si>
-  <si>
     <t>MO (Freetext)</t>
   </si>
   <si>
@@ -139,15 +130,6 @@
     <t>19D</t>
   </si>
   <si>
-    <t>Narrative content</t>
-  </si>
-  <si>
-    <t>CH1/001/2024</t>
-  </si>
-  <si>
-    <t>Convicted</t>
-  </si>
-  <si>
     <t>Number of Suspects</t>
   </si>
   <si>
@@ -190,15 +172,6 @@
     <t>CCTV Reviewed</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Victim Ethnicity</t>
   </si>
   <si>
@@ -232,9 +205,6 @@
     <t>Victim Last Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Name </t>
-  </si>
-  <si>
     <t>12/12345/A</t>
   </si>
   <si>
@@ -265,9 +235,6 @@
     <t>Location Type</t>
   </si>
   <si>
-    <t>Public / Private</t>
-  </si>
-  <si>
     <t>Suspect First Name</t>
   </si>
   <si>
@@ -308,6 +275,162 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Jon</t>
+  </si>
+  <si>
+    <t>Jack Bauer</t>
+  </si>
+  <si>
+    <t>Under review - Looks like a dodgy decision</t>
+  </si>
+  <si>
+    <t>Refer back to Force to do better</t>
+  </si>
+  <si>
+    <t>Two males attacked two victims, raping them</t>
+  </si>
+  <si>
+    <t>Victim's did not support prosecution.  No CCTV, No witnesses.</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Maecenas tincidunt.</t>
+  </si>
+  <si>
+    <t>Nil</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Natalie</t>
+  </si>
+  <si>
+    <t>Elizabeth</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>NR6 7LW</t>
+  </si>
+  <si>
+    <t>14/12345/A</t>
+  </si>
+  <si>
+    <t>14/12345</t>
+  </si>
+  <si>
+    <t>NR18 0WW</t>
+  </si>
+  <si>
+    <t>Fred</t>
+  </si>
+  <si>
+    <t>Purves</t>
+  </si>
+  <si>
+    <t>15/12336/P</t>
+  </si>
+  <si>
+    <t>14/8585</t>
+  </si>
+  <si>
+    <t>Jessica Fletcher</t>
+  </si>
+  <si>
+    <t>37/23456/25</t>
+  </si>
+  <si>
+    <t>Reviewed - correct decision</t>
+  </si>
+  <si>
+    <t>They did everything right!</t>
+  </si>
+  <si>
+    <t>Private</t>
+  </si>
+  <si>
+    <t>IP1 1AN</t>
+  </si>
+  <si>
+    <t>Two men, known to the three victims, raped them</t>
+  </si>
+  <si>
+    <t>NFA'd due to lack of forensic and digital evidence supporting</t>
+  </si>
+  <si>
+    <t>N MG3</t>
+  </si>
+  <si>
+    <t>NIL</t>
+  </si>
+  <si>
+    <t>BPORT/001/2024</t>
+  </si>
+  <si>
+    <t>BPORT/002/2024</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Sophie</t>
+  </si>
+  <si>
+    <t>Edger</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>11/13/1999</t>
+  </si>
+  <si>
+    <t>16/55555/K</t>
+  </si>
+  <si>
+    <t>16/4286</t>
+  </si>
+  <si>
+    <t>IP1 1AX</t>
+  </si>
+  <si>
+    <t>IP1 1BA</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>Guy</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t>Settled Status</t>
+  </si>
+  <si>
+    <t>IP1 1BH</t>
+  </si>
+  <si>
+    <t>IP1 1AU</t>
   </si>
 </sst>
 </file>
@@ -336,10 +459,12 @@
       <family val="2"/>
     </font>
     <font>
+      <i/>
       <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <color rgb="FF0070C0"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -362,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -380,6 +505,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -722,7 +857,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="J3" dT="2025-09-03T09:43:53.04" personId="{F6F4A7E9-6C7D-4895-A590-1552A97E093C}" id="{311A7AA6-15CF-4FD5-9E87-9BAE24BC9A3F}">
+  <threadedComment ref="I2" dT="2025-09-03T09:43:53.04" personId="{F6F4A7E9-6C7D-4895-A590-1552A97E093C}" id="{311A7AA6-15CF-4FD5-9E87-9BAE24BC9A3F}">
     <text xml:space="preserve">For text analysis (key words, thematic analysis etc)
 </text>
   </threadedComment>
@@ -734,64 +869,83 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="B1:G3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="3">
+        <v>36</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>106</v>
+      </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="3">
-        <v>36</v>
+        <v>95</v>
+      </c>
+      <c r="C3" s="3">
+        <v>37</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>14</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="G3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -803,126 +957,171 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B1:P3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="N1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="5" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="6">
+        <v>41761</v>
+      </c>
+      <c r="C2" s="6">
+        <v>42127</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P2" s="1" t="s">
+      <c r="E2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="2:16" s="5" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="6">
-        <v>45292</v>
-      </c>
-      <c r="D3" s="6">
-        <v>45292</v>
+      <c r="G2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" s="6">
+        <v>42170</v>
+      </c>
+      <c r="M2" s="5">
+        <v>14</v>
+      </c>
+      <c r="N2" s="6">
+        <v>42171</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="10" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="9">
+        <v>42527</v>
+      </c>
+      <c r="C3" s="9">
+        <v>44123</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>20</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="6">
-        <v>45717</v>
-      </c>
-      <c r="N3" s="5">
-        <v>1</v>
-      </c>
-      <c r="O3" s="6">
-        <v>45746</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="L3" s="9">
+        <v>44129</v>
+      </c>
+      <c r="M3" s="10">
+        <v>14</v>
+      </c>
+      <c r="N3" s="9">
+        <v>45955</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -936,139 +1135,190 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="B1:R3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="2:18" s="5" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
-        <v>10</v>
+    </row>
+    <row r="2" spans="1:17" s="5" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="5">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5">
+        <v>0</v>
+      </c>
+      <c r="L2" s="5">
+        <v>0</v>
+      </c>
+      <c r="M2" s="5">
+        <v>0</v>
+      </c>
+      <c r="N2" s="5">
+        <v>0</v>
+      </c>
+      <c r="O2" s="5">
+        <v>0</v>
+      </c>
+      <c r="P2" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="5" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
       </c>
       <c r="C3" s="5">
         <v>2</v>
       </c>
       <c r="D3" s="5">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5">
         <v>2</v>
       </c>
-      <c r="E3" s="5">
+      <c r="I3" s="5">
         <v>3</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="J3" s="5">
-        <v>4</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>43</v>
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
+        <v>0</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0</v>
+      </c>
+      <c r="N3" s="5">
+        <v>0</v>
+      </c>
+      <c r="O3" s="5">
+        <v>1</v>
+      </c>
+      <c r="P3" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1081,105 +1331,204 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="B1:M3"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="40.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="38.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="40.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:12" s="3" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="4">
+        <v>36526</v>
+      </c>
+      <c r="F2" s="3">
+        <v>15</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="4">
+        <v>36527</v>
+      </c>
+      <c r="F3" s="3">
+        <v>15</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="J3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F4" s="3">
+        <v>16</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5" s="3">
+        <v>44302</v>
+      </c>
+      <c r="F5" s="3">
+        <v>14</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13" s="3" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="4">
-        <v>36526</v>
-      </c>
-      <c r="G3" s="3">
-        <v>15</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>63</v>
+      <c r="L5" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1192,111 +1541,220 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="B1:N3"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="42.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="39.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="4">
+        <v>27426</v>
+      </c>
+      <c r="F2" s="3">
+        <v>40</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="M2" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="4">
+        <v>27455</v>
+      </c>
+      <c r="F3" s="3">
+        <v>40</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="4">
+        <v>35950</v>
+      </c>
+      <c r="F4" s="3">
+        <v>18</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="4">
-        <v>34700</v>
-      </c>
-      <c r="G3" s="3">
-        <v>20</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>63</v>
+      <c r="K4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="4">
+        <v>36322</v>
+      </c>
+      <c r="F5" s="3">
+        <v>17</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>